<commit_message>
Alteração das histórias de usuário para adequação ao padrão desejado / alteração do diagrama de casos de uso para se adequar a solução atual do projeto
</commit_message>
<xml_diff>
--- a/Desenvolvimento/4.Teste/AGP - Roteiro de Testes 1.1.xlsx
+++ b/Desenvolvimento/4.Teste/AGP - Roteiro de Testes 1.1.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\AGP\Desenvolvimento\4.Teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35B069A-39D1-4F4B-B2C6-64745DDAE996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52856D0A-8833-45CE-9730-6B0B15782AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="913" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8580" yWindow="3525" windowWidth="21600" windowHeight="11205" tabRatio="913" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
     <sheet name="AUX" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="UC01" sheetId="3" r:id="rId3"/>
-    <sheet name="UC03" sheetId="28" r:id="rId4"/>
-    <sheet name="UC04" sheetId="33" r:id="rId5"/>
-    <sheet name="UC05" sheetId="32" r:id="rId6"/>
-    <sheet name="UC06" sheetId="31" r:id="rId7"/>
-    <sheet name="UC07" sheetId="30" r:id="rId8"/>
-    <sheet name="UC08" sheetId="29" r:id="rId9"/>
-    <sheet name="UC09" sheetId="35" r:id="rId10"/>
+    <sheet name="UC02" sheetId="36" r:id="rId4"/>
+    <sheet name="UC03" sheetId="28" r:id="rId5"/>
+    <sheet name="UC04" sheetId="33" r:id="rId6"/>
+    <sheet name="UC05" sheetId="32" r:id="rId7"/>
+    <sheet name="UC06" sheetId="31" r:id="rId8"/>
+    <sheet name="UC07" sheetId="30" r:id="rId9"/>
+    <sheet name="UC08" sheetId="29" r:id="rId10"/>
+    <sheet name="UC09" sheetId="35" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="___xlfn_IFERROR">NA()</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -312,6 +313,18 @@
   </si>
   <si>
     <t>Aluno consegue visualizar todas os avisos de suas respectivas matérias</t>
+  </si>
+  <si>
+    <t>UC02 - Visualizar Matérias</t>
+  </si>
+  <si>
+    <t>Caso de uso não foi trazido para a versão final do projeto, como descrito na planilha de controle e planejamento do projeto.</t>
+  </si>
+  <si>
+    <t>Marcar como pendente</t>
+  </si>
+  <si>
+    <t>A atividade é marcada como pendente e desaparece da aba concluídas</t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1487,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1606,7 +1619,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -1721,7 +1734,7 @@
       </c>
       <c r="D21" s="22">
         <f>SUM(D5:D19)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F21" s="3">
         <f>SUM(F5:F19)</f>
@@ -1767,12 +1780,296 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC6D9D-36DD-4683-8961-B6967A3741D3}">
+  <dimension ref="A1:W19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="37">
+        <v>4</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>6</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F67FD7A-1F5F-4B1D-86BC-1995A2C10E53}">
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2075,7 +2372,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2354,12 +2651,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576B397A-3A91-41DD-AA50-32F9E4528128}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F838BA-2D88-48D5-BFEC-D6D94675F67D}">
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2382,14 +2679,14 @@
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -2406,9 +2703,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
@@ -2416,7 +2711,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="16" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2443,1119 +2738,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-    </row>
-    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-    </row>
-    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:B4"/>
-  </mergeCells>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D76902-9B12-4E75-A08B-1AF2D08CBF5E}">
-  <dimension ref="A1:W19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
-    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-    </row>
-    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="37">
-        <v>2</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-    </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-    </row>
-    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-    </row>
-    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:B4"/>
-  </mergeCells>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2866E4-F731-41AA-A6A5-2F63A70A7BFB}">
-  <dimension ref="A1:W19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
-    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-    </row>
-    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="37">
-        <v>2</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-    </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-    </row>
-    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-    </row>
-    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:B4"/>
-  </mergeCells>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7329EF34-3F3E-49A3-8AAA-677C2250E6A9}">
-  <dimension ref="A1:W19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
-    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-    </row>
-    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="37">
-        <v>2</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-    </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-    </row>
-    <row r="10" spans="1:23" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-    </row>
-    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:B4"/>
-  </mergeCells>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4773F568-F9CC-4800-9C7D-58BCB597A5F9}">
-  <dimension ref="A1:W19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
-    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-    </row>
-    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="37">
-        <v>1</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-    </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="9" spans="1:23" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>70</v>
-      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -3719,13 +2908,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC6D9D-36DD-4683-8961-B6967A3741D3}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576B397A-3A91-41DD-AA50-32F9E4528128}">
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3755,7 +2944,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -3773,7 +2962,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="15" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3814,13 +3003,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -3847,13 +3036,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -3880,13 +3069,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -3897,14 +3086,1102 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>79</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>6</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D76902-9B12-4E75-A08B-1AF2D08CBF5E}">
+  <dimension ref="A1:W19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="37">
+        <v>2</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>6</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2866E4-F731-41AA-A6A5-2F63A70A7BFB}">
+  <dimension ref="A1:W19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="37">
+        <v>2</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>6</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7329EF34-3F3E-49A3-8AAA-677C2250E6A9}">
+  <dimension ref="A1:W19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="37">
+        <v>2</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>6</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4773F568-F9CC-4800-9C7D-58BCB597A5F9}">
+  <dimension ref="A1:W19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="37">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>

</xml_diff>